<commit_message>
adding in tests for check data format function
</commit_message>
<xml_diff>
--- a/inst/extdata/demo-template-fish-exploit.xlsx
+++ b/inst/extdata/demo-template-fish-exploit.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aylapearson/Code/chktemplate/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49D2F313-40BA-9E44-9D59-ABC157FB792A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D891F5D3-8390-0A4C-86DB-C978D397DB8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28020" yWindow="3020" windowWidth="27720" windowHeight="17040" xr2:uid="{D2F727D3-E3E6-DE42-943C-87973B24BE7C}"/>
+    <workbookView xWindow="1340" yWindow="760" windowWidth="32840" windowHeight="11380" activeTab="2" xr2:uid="{D2F727D3-E3E6-DE42-943C-87973B24BE7C}"/>
   </bookViews>
   <sheets>
-    <sheet name="outing" sheetId="2" r:id="rId1"/>
-    <sheet name="capture" sheetId="1" r:id="rId2"/>
-    <sheet name="recapture" sheetId="3" r:id="rId3"/>
+    <sheet name="site" sheetId="4" r:id="rId1"/>
+    <sheet name="outing" sheetId="2" r:id="rId2"/>
+    <sheet name="capture" sheetId="1" r:id="rId3"/>
+    <sheet name="recapture" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="83">
   <si>
     <t>year</t>
   </si>
@@ -272,6 +273,18 @@
   </si>
   <si>
     <t>c(0, 10)</t>
+  </si>
+  <si>
+    <t>site</t>
+  </si>
+  <si>
+    <t>site_name</t>
+  </si>
+  <si>
+    <t>Bendy Bay</t>
+  </si>
+  <si>
+    <t>name of the site</t>
   </si>
 </sst>
 </file>
@@ -630,153 +643,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D07577A-358A-F34F-9161-33686BFF2FB9}">
-  <dimension ref="A1:J7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41F9F3AD-6970-E249-AFD5-254D3E0D5ED0}">
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="19.83203125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>35</v>
       </c>
       <c r="B1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>2015</v>
-      </c>
-      <c r="D2">
-        <v>7</v>
-      </c>
-      <c r="E2">
-        <v>14</v>
-      </c>
-      <c r="F2">
-        <v>9</v>
-      </c>
-      <c r="G2">
-        <v>30</v>
-      </c>
-      <c r="H2" t="s">
-        <v>72</v>
-      </c>
-      <c r="I2">
-        <v>4</v>
-      </c>
-      <c r="J2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I3" t="s">
-        <v>32</v>
-      </c>
-      <c r="J3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G4" t="s">
-        <v>59</v>
-      </c>
-      <c r="H4" t="s">
-        <v>73</v>
-      </c>
-      <c r="I4" t="s">
-        <v>78</v>
-      </c>
-      <c r="J4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -784,15 +692,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>69</v>
       </c>
@@ -803,29 +708,222 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA9B9C42-9339-A047-901C-9A85D8DE94F1}">
-  <dimension ref="A1:L7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D07577A-358A-F34F-9161-33686BFF2FB9}">
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20" customWidth="1"/>
+    <col min="10" max="10" width="19.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2">
+        <v>2015</v>
+      </c>
+      <c r="E2">
+        <v>7</v>
+      </c>
+      <c r="F2">
+        <v>14</v>
+      </c>
+      <c r="G2">
+        <v>9</v>
+      </c>
+      <c r="H2">
+        <v>30</v>
+      </c>
+      <c r="I2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J2">
+        <v>4</v>
+      </c>
+      <c r="K2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4" t="s">
+        <v>73</v>
+      </c>
+      <c r="J4" t="s">
+        <v>78</v>
+      </c>
+      <c r="K4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA9B9C42-9339-A047-901C-9A85D8DE94F1}">
+  <dimension ref="A1:M7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="32" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="32" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -833,75 +931,81 @@
         <v>49</v>
       </c>
       <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2">
         <v>10</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>42</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>523012</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>5497670</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>29</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>510</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>5.2</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>14</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>72</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -909,37 +1013,40 @@
         <v>50</v>
       </c>
       <c r="C3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" t="s">
         <v>23</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>20</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>21</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>22</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>24</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>25</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>26</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>42</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>43</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -947,37 +1054,40 @@
         <v>66</v>
       </c>
       <c r="C4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" t="s">
         <v>58</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>59</v>
-      </c>
-      <c r="E4" t="s">
-        <v>67</v>
       </c>
       <c r="F4" t="s">
         <v>67</v>
       </c>
       <c r="G4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H4" t="s">
         <v>74</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>66</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>61</v>
-      </c>
-      <c r="J4" t="s">
-        <v>75</v>
       </c>
       <c r="K4" t="s">
         <v>75</v>
       </c>
       <c r="L4" t="s">
+        <v>75</v>
+      </c>
+      <c r="M4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -990,20 +1100,26 @@
       <c r="D5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="J6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>69</v>
       </c>
       <c r="B7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1012,7 +1128,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5014DBCF-9011-9A47-9D03-DDE81D462BF0}">
   <dimension ref="A1:O6"/>
   <sheetViews>

</xml_diff>

<commit_message>
update template fixes #12
</commit_message>
<xml_diff>
--- a/inst/extdata/demo-template-fish-exploit.xlsx
+++ b/inst/extdata/demo-template-fish-exploit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aylapearson/Code/chktemplate/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90B51BCF-EEF9-C24E-892A-3F66A7361C49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24969668-4280-0B4D-8111-E5BC72F013F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="760" windowWidth="32840" windowHeight="11380" xr2:uid="{D2F727D3-E3E6-DE42-943C-87973B24BE7C}"/>
+    <workbookView xWindow="-35360" yWindow="2320" windowWidth="32840" windowHeight="11380" activeTab="3" xr2:uid="{D2F727D3-E3E6-DE42-943C-87973B24BE7C}"/>
   </bookViews>
   <sheets>
     <sheet name="site" sheetId="4" r:id="rId1"/>
@@ -646,7 +646,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41F9F3AD-6970-E249-AFD5-254D3E0D5ED0}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -712,7 +712,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -874,16 +874,10 @@
       <c r="B5" t="b">
         <v>1</v>
       </c>
-      <c r="I5" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
-      </c>
-      <c r="F6" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -904,7 +898,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1103,6 +1097,9 @@
       <c r="E5" t="b">
         <v>1</v>
       </c>
+      <c r="K5" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -1132,8 +1129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5014DBCF-9011-9A47-9D03-DDE81D462BF0}">
   <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1256,15 +1253,6 @@
       <c r="A5" t="s">
         <v>63</v>
       </c>
-      <c r="B5" t="b">
-        <v>1</v>
-      </c>
-      <c r="C5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D5" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -1275,9 +1263,7 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="1" t="b">
-        <v>1</v>
-      </c>
+      <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>

</xml_diff>

<commit_message>
update the demo templates a bit more
</commit_message>
<xml_diff>
--- a/inst/extdata/demo-template-fish-exploit.xlsx
+++ b/inst/extdata/demo-template-fish-exploit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aylapearson/Code/chktemplate/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24969668-4280-0B4D-8111-E5BC72F013F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8D9B37-D5B6-B948-B08E-700C82C31D44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35360" yWindow="2320" windowWidth="32840" windowHeight="11380" activeTab="3" xr2:uid="{D2F727D3-E3E6-DE42-943C-87973B24BE7C}"/>
+    <workbookView xWindow="-35360" yWindow="2320" windowWidth="32840" windowHeight="11380" activeTab="2" xr2:uid="{D2F727D3-E3E6-DE42-943C-87973B24BE7C}"/>
   </bookViews>
   <sheets>
     <sheet name="site" sheetId="4" r:id="rId1"/>
@@ -647,7 +647,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -695,6 +695,9 @@
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
+      </c>
+      <c r="B6" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -712,7 +715,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -879,6 +882,9 @@
       <c r="A6" t="s">
         <v>16</v>
       </c>
+      <c r="B6" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -897,8 +903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA9B9C42-9339-A047-901C-9A85D8DE94F1}">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1108,6 +1114,9 @@
       <c r="K6" t="b">
         <v>1</v>
       </c>
+      <c r="L6" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -1129,7 +1138,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5014DBCF-9011-9A47-9D03-DDE81D462BF0}">
   <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
remove guide from join in capture table
</commit_message>
<xml_diff>
--- a/inst/extdata/demo-template-fish-exploit.xlsx
+++ b/inst/extdata/demo-template-fish-exploit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aylapearson/Code/chktemplate/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8D9B37-D5B6-B948-B08E-700C82C31D44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4556AE35-DF50-9F45-8FF0-55379E10231A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-35360" yWindow="2320" windowWidth="32840" windowHeight="11380" activeTab="2" xr2:uid="{D2F727D3-E3E6-DE42-943C-87973B24BE7C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="83">
   <si>
     <t>year</t>
   </si>
@@ -715,7 +715,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B5" sqref="B5:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -903,8 +903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA9B9C42-9339-A047-901C-9A85D8DE94F1}">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1123,9 +1123,6 @@
         <v>82</v>
       </c>
       <c r="B7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>